<commit_message>
feat: Finalize compliance pipeline with robust rule-based checks, updated ground truth, and comprehensive docs
</commit_message>
<xml_diff>
--- a/docs/uyum_denetim_raporu.xlsx
+++ b/docs/uyum_denetim_raporu.xlsx
@@ -5303,12 +5303,12 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>Banka 25 TL hesap işletim ücreti alıyor. Tebliğ'de bu ücret için bir limit belirtilmemiş olsa da, Ek-1 listesinde yer almıyor. Bu durumda, Tebliğ'in genel yasaklama hükmüne göre, bu ücretin alınması yasaktır.</t>
+          <t>Banka 25 TL hesap işletim ücreti alıyor. Ek-1 listesinde hesap işletim ücreti belirtilmemiş ve bu ücretin alınması yasaktır. Tebliğ'de açıkça yasaklanmış bir ücret alınmaktadır.</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>Madde 11/Fıkra 1, Madde 11/Fıkra 6, Madde 6/Fıkra 1, Madde 6/Fıkra 2, Madde 9/Fıkra 1, Madde 9/Fıkra 6, Madde Ek-1/Fıkra Tam Liste</t>
+          <t>Madde 11/Fıkra 1, Madde 9/Fıkra 1, Madde Ek-1/Fıkra Tam Liste</t>
         </is>
       </c>
       <c r="G132" t="inlineStr">
@@ -5340,7 +5340,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>Banka kendi ATM'sinden para çekme işleminden 5.0 TL ücret alıyor. Tebliğ'e göre kendi ATM'lerinden para çekme işlemlerinden ücret alınamaz. Bu durum Tebliğ'in açıkça yasakladığı bir durumu ihlal etmektedir.</t>
+          <t>Banka kendi ATM'sinden para çekme işleminden 5 TL ücret alıyor. Tebliğ'e göre kendi ATM'lerinden para çekme işlemlerinden ücret alınamaz. Bu durum Tebliğ'in açıkça yasakladığı bir durumu içeriyor.</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -5372,22 +5372,22 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>NOT_OK</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>Banka 15 TL ücret alıyor. Ek-1 listesinde 'Başka Kuruluş ATM'sinden Yapılan İşlem Ücreti' yer alıyor. Ancak, bu maddeye ilişkin Tebliğ'de sayısal bir limit belirtilmemiştir. Bu nedenle, Ek-1'de yer almasına rağmen, sayısal bir limit olmaması nedeniyle ihlal durumu söz konusudur.</t>
+          <t>Banka maddesi 'Başka Banka ATM Nakit Çekim' ücretinden bahsediyor. Ek-1 listesinde 'Başka Kuruluş ATM'sinden Yapılan İşlem Ücreti' yer alıyor. Bu, ücretin izin verildiği anlamına gelir. Ancak, Tebliğ'de bu işlem için bir sayısal limit belirtilmemiştir. Bu nedenle, ihlal olup olmadığını belirlemek mümkün değildir. Bu durumda NA vermek en doğru yaklaşımdır.</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>Madde 11/Fıkra 3, Madde 6/Fıkra 1, Madde 6/Fıkra 2, Madde 9/Fıkra 6, Madde Ek-1/Fıkra Tam Liste</t>
+          <t>Madde 6/Fıkra 1, Madde 6/Fıkra 2, Madde 9/Fıkra 6, Madde Ek-1/Fıkra Tam Liste</t>
         </is>
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>Başka Banka ATM'sinden yapılan işlem ücreti, ilgili mevzuatta belirtilen azami tutarı aşamaz.</t>
+          <t>Gerekli Değil</t>
         </is>
       </c>
     </row>
@@ -5419,7 +5419,7 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>Madde 6/Fıkra 1, Madde 6/Fıkra 2, Madde 9/Fıkra 1, Madde 9/Fıkra 6, Madde Ek-1/Fıkra Tam Liste</t>
+          <t>Madde 6/Fıkra 1, Madde 6/Fıkra 2, Madde Ek-1/Fıkra Tam Liste</t>
         </is>
       </c>
       <c r="G135" t="inlineStr">
@@ -5451,12 +5451,12 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Banka 15.0 TL EFT ücreti alıyor, ancak Tebliğ'e göre 1000-50000 TL arası EFT ücreti 10.0 TL'yi geçemez. 5.0 TL fazla ücret alınmıştır.</t>
+          <t>Banka 15.0 TL şube EFT ücreti alıyor, ancak Tebliğ'e göre 10.0 TL'yi geçemiyor. 5.0 TL fazla ücret alınıyor.</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Madde 11/Fıkra 6, Madde 6/Fıkra 1, Madde 6/Fıkra 2, Madde 9/Fıkra 1, Madde Ek-1/Fıkra Tam Liste</t>
+          <t>Madde 11/Fıkra 6, Madde 9/Fıkra 1, Madde Ek-1/Fıkra Tam Liste</t>
         </is>
       </c>
       <c r="G136" t="inlineStr">
@@ -5488,17 +5488,17 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Banka 50 TL hesap açılış ücreti alıyor. Tebliğ'e göre mevduat ve katılım fonu hesaplarının açılış işlemlerinde ücret alınamaz. Bu, açık bir ücret yasaklamasıdır.</t>
+          <t>Banka 50.0 TL hesap açılış ücreti alıyor. Tebliğ'in 13. maddesinin 1. fıkrası, mevduat ve katılım fonu hesaplarının açılış işlemlerinde ücret alınamayacağını belirtiyor. Bu durum, Tebliğ'e aykırıdır.</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>Madde 12/Fıkra 2, Madde 12/Fıkra 3, Madde 13/Fıkra 1, Madde 6/Fıkra 1, Madde 6/Fıkra 2, Madde 9/Fıkra 1, Madde 9/Fıkra 6, Madde Ek-1/Fıkra Tam Liste</t>
+          <t>Madde 12/Fıkra 2, Madde 12/Fıkra 3, Madde 13/Fıkra 1, Madde 6/Fıkra 2, Madde Ek-1/Fıkra Tam Liste</t>
         </is>
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>Hesap açılışında herhangi bir ücret alınmayacaktır.</t>
+          <t>Hesap açılış işlemlerinde herhangi bir ücret alınmayacaktır.</t>
         </is>
       </c>
     </row>
@@ -5525,12 +5525,12 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Banka 15 TL hesap bakım ücreti alıyor. Tebliğ'e göre mevduat ve katılım fonu hesaplarından hesap işletim ücreti alınamaz. Bu durum, Tebliğ'deki yasağa aykırıdır.</t>
+          <t>Banka 15 TL hesap bakım ücreti alıyor. Tebliğ'e göre mevduat hesaplarından hesap işletim ücreti alınamaz. Bu durum, Tebliğ'in açıkça yasakladığı bir ücretlendirme uygulamasıdır.</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>Madde 11/Fıkra 1, Madde 11/Fıkra 6, Madde 6/Fıkra 1, Madde 6/Fıkra 2, Madde 9/Fıkra 6, Madde Ek-1/Fıkra Tam Liste</t>
+          <t>Madde 11/Fıkra 1, Madde 9/Fıkra 1, Madde Ek-1/Fıkra Tam Liste</t>
         </is>
       </c>
       <c r="G138" t="inlineStr">
@@ -5562,12 +5562,12 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Banka SMS bilgilendirme hizmeti için 10 TL ücret alıyor. Tebliğ'de bu hizmetin ücretsiz olması gerektiğine dair bir hüküm bulunmamakla birlikte, SMS bilgilendirme hizmeti zorunlu olduğu için ücret alınması yasaktır. Ek-1 listesinde de bu ücret kalemi yer almamaktadır.</t>
+          <t>Banka SMS bilgilendirme hizmeti için 10 TL ücret alıyor. Tebliğ'de bu hizmetin ücretsiz olması gerekmektedir. Ek-1 listesinde SMS bilgilendirme ücreti yer almamaktadır. Bu nedenle ücret alınması yasaktır.</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>Madde 11/Fıkra 6, Madde 6/Fıkra 2, Madde 9/Fıkra 1, Madde 9/Fıkra 5, Madde Ek-1/Fıkra Tam Liste</t>
+          <t>Madde 11/Fıkra 6, Madde 9/Fıkra 1, Madde 9/Fıkra 5, Madde Ek-1/Fıkra Tam Liste</t>
         </is>
       </c>
       <c r="G139" t="inlineStr">
@@ -5599,12 +5599,12 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Banka 5.0 TL ücret alıyor, Tebliğde bu hizmetin ücretsiz olması gerektiği belirtiliyor. Ücretsiz olması gereken bir işlem için ücret alınması Tebliğ'e aykırıdır.</t>
+          <t>Banka, E-posta bilgilendirme hizmeti için 5.0 TL ücret alıyor. Tebliğ'de bu hizmetin ücretsiz olması gerektiği belirtilmiyor ancak Ek-1 listesinde izin verilen ücret kalemleri arasında yer almıyor. Bu nedenle, ücretsiz olması gereken bir hizmet için ücret alınması Tebliğ'e aykırıdır.</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>Madde 11/Fıkra 6, Madde 6/Fıkra 1, Madde 9/Fıkra 1, Madde 9/Fıkra 5, Madde Ek-1/Fıkra Tam Liste</t>
+          <t>Madde 11/Fıkra 6, Madde 9/Fıkra 1, Madde 9/Fıkra 5, Madde Ek-1/Fıkra Tam Liste</t>
         </is>
       </c>
       <c r="G140" t="inlineStr">
@@ -5636,17 +5636,17 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Banka, SMS bildirimi için 8.0 TL ücret alıyor. Tebliğ'de bu hizmet için ücret alınamayacağına dair bir hüküm bulunmamakla birlikte, Ek-1 listesinde de yer almıyor. Bu durum, Tebliğ'de belirtilen izin verilmeyen ücretlerin alınması yasağına aykırıdır.</t>
+          <t>Banka, müşteri onayı olmadan SMS bildirimi için ücret alıyor. Tebliğ, müşteri onayı gerektiren işlemler için açıkça izin vermiyor ve bu durum müşteri haklarının ihlali anlamına gelir. Bu, müşteri onayı olmadan ücret alınması yasağına aykırıdır.</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>Madde 11/Fıkra 6, Madde 6/Fıkra 1, Madde 6/Fıkra 2, Madde 9/Fıkra 1, Madde Ek-1/Fıkra Tam Liste</t>
+          <t>Madde 11/Fıkra 6, Madde 6/Fıkra 2, Madde Ek-1/Fıkra Tam Liste</t>
         </is>
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>Müşteri onayı olmadan SMS bildirimi hizmeti için ücret alınamaz.</t>
+          <t>Müşteri onayı alınmadan SMS bildirimi gönderilemez. Müşteri onayı alındıktan sonra belirtilen ücret tahsil edilebilir.</t>
         </is>
       </c>
     </row>
@@ -5673,17 +5673,17 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>Banka kendi hesabına para yatırma işleminden 3 TL ücret alıyor. Tebliğ'e göre kendi hesabına para yatırma işlemlerinden ücret alınamaz. Bu durum Tebliğ'in ilgili maddesini ihlal etmektedir.</t>
+          <t>Banka kendi hesabına para yatırma işleminden 3 TL ücret alıyor. Tebliğ'e göre kendi hesabına para yatırma işlemlerinden ücret alınamaz. Bu durum, Tebliğ'in açıkça yasakladığı bir durumu ihlal etmektedir.</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>Madde 6/Fıkra 1, Madde 6/Fıkra 2, Madde 9/Fıkra 1, Madde 9/Fıkra 6, Madde Ek-1/Fıkra Tam Liste</t>
+          <t>Madde 9/Fıkra 1, Madde Ek-1/Fıkra Tam Liste</t>
         </is>
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>Kendi hesabına para yatırma işlemlerinden ücret alınamaz.</t>
+          <t>Kendi hesabına para yatırma işlemleri ücretsizdir.</t>
         </is>
       </c>
     </row>
@@ -5710,17 +5710,17 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Banka 25.0 TL ücret alıyor, ancak Tebliğ'de bu hizmet için herhangi bir ücret alınmaması gerektiği belirtilmektedir. Bu durum, Tebliğ'in yasaklama hükmünü ihlal etmektedir.</t>
+          <t>Banka, sözleşme ilk yıl içinde tekrar basımı için 25 TL ücret alıyor. Tebliğ'e göre sözleşmenin bir örneği ilk yıl ücretsiz verilmesi zorunludur. Bu durum, Tebliğ'in [MADDE 9 - FIKRA 4] hükmünü ihlal etmektedir.</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>Madde 9/Fıkra 3, Madde 9/Fıkra 4, Madde 9/Fıkra 6, Madde Ek-1/Fıkra Tam Liste</t>
+          <t>Madde 9/Fıkra 3, Madde Ek-1/Fıkra Tam Liste</t>
         </is>
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>Hizmet Türü: Sözleşme İlk Yıl İçinde Tekrar Basımı. Ücret: 0 TL</t>
+          <t>Sözleşme örneği ilk yıl ücretsizdir.</t>
         </is>
       </c>
     </row>

</xml_diff>